<commit_message>
change name of latin species col of mammal requirements to Species_latin
</commit_message>
<xml_diff>
--- a/Mammal_requirements.xlsx
+++ b/Mammal_requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18274077-389E-0447-BD58-8D19BF60B834}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1FB7C7-9232-A14F-9992-7670BAF82671}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1580" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="143">
   <si>
     <t>Species</t>
   </si>
@@ -460,6 +460,9 @@
   </si>
   <si>
     <t>Nesting habitat</t>
+  </si>
+  <si>
+    <t>Species_latin</t>
   </si>
 </sst>
 </file>
@@ -585,6 +588,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,15 +607,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -948,7 +951,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -984,76 +987,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="18" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="19" t="s">
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="23" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="24" t="s">
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
       <c r="Z2" s="7" t="s">
         <v>126</v>
       </c>
@@ -1066,29 +1069,29 @@
       <c r="AC2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="AD2" s="20" t="s">
+      <c r="AD2" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="21" t="s">
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="20" t="s">
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="21" t="s">
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="AK2" s="21"/>
+      <c r="AK2" s="24"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>89</v>
@@ -6214,17 +6217,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E1:Y1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:Y2"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AD1:AK1"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="E1:Y1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>